<commit_message>
completed laporan print & xlsx
</commit_message>
<xml_diff>
--- a/public_html/Sales By Customer Detail.xlsx
+++ b/public_html/Sales By Customer Detail.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
   <si>
     <t>Customer</t>
   </si>
@@ -42,6 +42,33 @@
   </si>
   <si>
     <t>Amount</t>
+  </si>
+  <si>
+    <t>CV. Susah MoveOn</t>
+  </si>
+  <si>
+    <t>SO/VH/030621 11:46:15/00001</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Nama Liquid</t>
+  </si>
+  <si>
+    <t>06-03-2021</t>
+  </si>
+  <si>
+    <t>Alacarte - Cream Biscuit By Jnc</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>Total Invoice</t>
+  </si>
+  <si>
+    <t>Total for CV. Susah MoveOn</t>
   </si>
   <si>
     <t>TOTAL</t>
@@ -386,10 +413,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -427,12 +454,88 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2"/>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
+        <v>225000</v>
+      </c>
       <c r="I2" s="1">
+        <v>225000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4"/>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>190000</v>
+      </c>
+      <c r="I4" s="1">
+        <v>190000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1">
         <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1">
+        <v>415000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1">
+        <v>415000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="1">
+        <v>415000</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <mergeCells>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="B7:I7"/>
+  </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>

</xml_diff>